<commit_message>
CartMaster CountryMaster and CurrancyMaster working fine 10 march 8:35pm
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/Countray Master.xlsx
+++ b/src/main/java/com/crm/qa/testdata/Countray Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devendra.singh1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devendra.singh1\git\Kargo360\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Country Code</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>THB</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,82 +464,82 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>